<commit_message>
feat: Normaliza e cria as tabelas necessárias
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>usuario_id</t>
   </si>
@@ -362,16 +362,82 @@
   <si>
     <t xml:space="preserve">79; 95; 213; 136; 83</t>
   </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>plans</t>
+  </si>
+  <si>
+    <t>plan_id</t>
+  </si>
+  <si>
+    <t>music_history</t>
+  </si>
+  <si>
+    <t>songs</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>music_history_id</t>
+  </si>
+  <si>
+    <t>songs_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>artist_id</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>album_name</t>
+  </si>
+  <si>
+    <t>release_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soul For Us</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
       <sz val="11.000000"/>
+    </font>
+    <font>
+      <name val="Helvetica Neue"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11.000000"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -386,15 +452,45 @@
       <sz val="11.000000"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="5"/>
+        <bgColor indexed="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5B95F9"/>
+        <bgColor rgb="FF5B95F9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F0FE"/>
+        <bgColor rgb="FFE8F0FE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -432,26 +528,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="48">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -478,16 +588,16 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -508,12 +618,79 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="2" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -1228,13 +1405,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="1" workbookViewId="0" zoomScale="113">
+    <sheetView showGridLines="0" showRowColHeaders="1" topLeftCell="A31" zoomScale="113" workbookViewId="0">
       <selection activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.5"/>
+    <col customWidth="1" min="1" max="1" width="23.7109375"/>
     <col customWidth="1" min="2" max="2" width="18.33203125"/>
     <col customWidth="1" min="3" max="3" width="16.5"/>
     <col customWidth="1" min="4" max="4" width="52.83203125"/>
@@ -1245,7 +1422,13 @@
     <col customWidth="1" min="9" max="9" width="14.5"/>
     <col customWidth="1" min="10" max="10" width="10.5"/>
     <col customWidth="1" min="11" max="11" width="20.5"/>
-    <col customWidth="1" min="12" max="26" width="8.83203125"/>
+    <col customWidth="1" min="12" max="12" width="8.83203125"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="15.00390625"/>
+    <col customWidth="1" min="14" max="15" width="8.83203125"/>
+    <col bestFit="1" customWidth="1" min="16" max="16" width="16.78125"/>
+    <col customWidth="1" min="17" max="17" width="8.83203125"/>
+    <col bestFit="1" customWidth="1" min="18" max="18" width="12.140625"/>
+    <col customWidth="1" min="19" max="26" width="8.83203125"/>
     <col customWidth="1" min="27" max="28" width="14.5"/>
   </cols>
   <sheetData>
@@ -1921,7 +2104,7 @@
       <c r="C15" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="25" t="s">
         <v>78</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -1962,7 +2145,7 @@
       <c r="C16" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="25" t="s">
         <v>83</v>
       </c>
       <c r="E16" s="22" t="s">
@@ -2003,7 +2186,7 @@
       <c r="C17" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="25" t="s">
         <v>88</v>
       </c>
       <c r="E17" s="22" t="s">
@@ -2044,7 +2227,7 @@
       <c r="C18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="25" t="s">
         <v>92</v>
       </c>
       <c r="E18" s="22" t="s">
@@ -2085,7 +2268,7 @@
       <c r="C19" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="26" t="s">
         <v>96</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -2126,7 +2309,7 @@
       <c r="C20" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="26" t="s">
         <v>101</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -2167,7 +2350,7 @@
       <c r="C21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="26" t="s">
         <v>105</v>
       </c>
       <c r="E21" s="19" t="s">
@@ -2208,7 +2391,7 @@
       <c r="C22" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="26" t="s">
         <v>109</v>
       </c>
       <c r="E22" s="19" t="s">
@@ -2249,7 +2432,7 @@
       <c r="C23" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="26" t="s">
         <v>114</v>
       </c>
       <c r="E23" s="19" t="s">
@@ -2371,10 +2554,12 @@
       <c r="AB26" s="5"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="A27" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -2401,10 +2586,18 @@
       <c r="AB27" s="5"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="A28" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -2431,10 +2624,18 @@
       <c r="AB28" s="5"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="A29" s="29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="29">
+        <v>23</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -2461,10 +2662,18 @@
       <c r="AB29" s="5"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="A30" s="31">
+        <v>2</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="31">
+        <v>35</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>19</v>
+      </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -2491,10 +2700,18 @@
       <c r="AB30" s="5"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="A31" s="29">
+        <v>3</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="29">
+        <v>20</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>26</v>
+      </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -2521,10 +2738,18 @@
       <c r="AB31" s="5"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
+      <c r="A32" s="31">
+        <v>4</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="31">
+        <v>45</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>33</v>
+      </c>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
@@ -2551,10 +2776,18 @@
       <c r="AB32" s="5"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
+      <c r="A33" s="29">
+        <v>5</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="29">
+        <v>58</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>39</v>
+      </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2581,10 +2814,18 @@
       <c r="AB33" s="5"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+      <c r="A34" s="31">
+        <v>6</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="31">
+        <v>33</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>44</v>
+      </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -2611,10 +2852,18 @@
       <c r="AB34" s="5"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+      <c r="A35" s="29">
+        <v>7</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="29">
+        <v>26</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>49</v>
+      </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -2641,10 +2890,18 @@
       <c r="AB35" s="5"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
+      <c r="A36" s="31">
+        <v>8</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="31">
+        <v>19</v>
+      </c>
+      <c r="D36" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -2671,10 +2928,18 @@
       <c r="AB36" s="5"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
+      <c r="A37" s="29">
+        <v>9</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="29">
+        <v>42</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>59</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -2701,10 +2966,18 @@
       <c r="AB37" s="5"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
+      <c r="A38" s="31">
+        <v>10</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="31">
+        <v>46</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>64</v>
+      </c>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -2761,9 +3034,11 @@
       <c r="AB39" s="5"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
+      <c r="A40" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -2791,9 +3066,15 @@
       <c r="AB40" s="5"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+      <c r="A41" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -2821,9 +3102,15 @@
       <c r="AB41" s="5"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+      <c r="A42" s="30">
+        <v>1</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="29">
+        <v>0</v>
+      </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -2851,9 +3138,15 @@
       <c r="AB42" s="5"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+      <c r="A43" s="32">
+        <v>2</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>20</v>
+      </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
@@ -2881,9 +3174,15 @@
       <c r="AB43" s="5"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
+      <c r="A44" s="30">
+        <v>3</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>27</v>
+      </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
@@ -2911,9 +3210,15 @@
       <c r="AB44" s="5"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
+      <c r="A45" s="32">
+        <v>4</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>34</v>
+      </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -2971,24 +3276,31 @@
       <c r="AB46" s="5"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
+      <c r="A47" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
+      <c r="F47" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="L47" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="M47" s="35"/>
       <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
+      <c r="O47" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="P47" s="35"/>
+      <c r="Q47" s="35"/>
+      <c r="R47" s="35"/>
       <c r="S47" s="11"/>
       <c r="T47" s="11"/>
       <c r="U47" s="11"/>
@@ -3001,24 +3313,53 @@
       <c r="AB47" s="5"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
+      <c r="A48" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="36" t="s">
+        <v>125</v>
+      </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
+      <c r="F48" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="I48" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="J48" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="L48" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="M48" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="N48" s="38"/>
+      <c r="O48" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="P48" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q48" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="R48" s="39" t="s">
+        <v>130</v>
+      </c>
       <c r="S48" s="11"/>
       <c r="T48" s="11"/>
       <c r="U48" s="11"/>
@@ -3037,18 +3378,32 @@
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="G49" s="11" t="s">
+        <v>131</v>
+      </c>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
+      <c r="L49" s="40">
+        <v>1</v>
+      </c>
+      <c r="M49" s="40" t="s">
+        <v>73</v>
+      </c>
       <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
+      <c r="O49" s="40">
+        <v>1</v>
+      </c>
+      <c r="P49" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q49" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="R49" s="42" t="s">
+        <v>76</v>
+      </c>
       <c r="S49" s="11"/>
       <c r="T49" s="11"/>
       <c r="U49" s="11"/>
@@ -3072,13 +3427,25 @@
       <c r="I50" s="11"/>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
+      <c r="L50" s="40">
+        <v>2</v>
+      </c>
+      <c r="M50" s="40" t="s">
+        <v>82</v>
+      </c>
       <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
+      <c r="O50" s="43">
+        <v>2</v>
+      </c>
+      <c r="P50" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q50" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="R50" s="45" t="s">
+        <v>80</v>
+      </c>
       <c r="S50" s="11"/>
       <c r="T50" s="11"/>
       <c r="U50" s="11"/>
@@ -3102,13 +3469,25 @@
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
+      <c r="L51" s="40">
+        <v>3</v>
+      </c>
+      <c r="M51" s="43" t="s">
+        <v>87</v>
+      </c>
       <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
+      <c r="O51" s="40">
+        <v>3</v>
+      </c>
+      <c r="P51" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q51" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="R51" s="42" t="s">
+        <v>85</v>
+      </c>
       <c r="S51" s="11"/>
       <c r="T51" s="11"/>
       <c r="U51" s="11"/>
@@ -3132,13 +3511,25 @@
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
+      <c r="L52" s="40">
+        <v>4</v>
+      </c>
+      <c r="M52" s="43" t="s">
+        <v>35</v>
+      </c>
       <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
+      <c r="O52" s="43">
+        <v>4</v>
+      </c>
+      <c r="P52" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q52" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="R52" s="45" t="s">
+        <v>90</v>
+      </c>
       <c r="S52" s="11"/>
       <c r="T52" s="11"/>
       <c r="U52" s="11"/>
@@ -3162,13 +3553,25 @@
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
+      <c r="L53" s="40">
+        <v>5</v>
+      </c>
+      <c r="M53" s="46" t="s">
+        <v>100</v>
+      </c>
       <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
+      <c r="O53" s="40">
+        <v>5</v>
+      </c>
+      <c r="P53" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q53" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="R53" s="42" t="s">
+        <v>94</v>
+      </c>
       <c r="S53" s="11"/>
       <c r="T53" s="11"/>
       <c r="U53" s="11"/>
@@ -3192,13 +3595,25 @@
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
+      <c r="L54" s="40">
+        <v>6</v>
+      </c>
+      <c r="M54" s="47" t="s">
+        <v>113</v>
+      </c>
       <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
+      <c r="O54" s="47">
+        <v>6</v>
+      </c>
+      <c r="P54" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q54" s="47">
+        <v>4</v>
+      </c>
+      <c r="R54" s="43" t="s">
+        <v>98</v>
+      </c>
       <c r="S54" s="11"/>
       <c r="T54" s="11"/>
       <c r="U54" s="11"/>
@@ -3222,13 +3637,19 @@
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
       <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
+      <c r="O55" s="46">
+        <v>7</v>
+      </c>
+      <c r="P55" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q55" s="46">
+        <v>5</v>
+      </c>
+      <c r="R55" s="40" t="s">
+        <v>103</v>
+      </c>
       <c r="S55" s="11"/>
       <c r="T55" s="11"/>
       <c r="U55" s="11"/>
@@ -3252,13 +3673,19 @@
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
       <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
+      <c r="O56" s="47">
+        <v>8</v>
+      </c>
+      <c r="P56" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q56" s="47">
+        <v>5</v>
+      </c>
+      <c r="R56" s="43" t="s">
+        <v>107</v>
+      </c>
       <c r="S56" s="11"/>
       <c r="T56" s="11"/>
       <c r="U56" s="11"/>
@@ -3282,13 +3709,19 @@
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
       <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
+      <c r="O57" s="46">
+        <v>9</v>
+      </c>
+      <c r="P57" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q57" s="46">
+        <v>5</v>
+      </c>
+      <c r="R57" s="40" t="s">
+        <v>111</v>
+      </c>
       <c r="S57" s="11"/>
       <c r="T57" s="11"/>
       <c r="U57" s="11"/>
@@ -3312,13 +3745,19 @@
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
       <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
+      <c r="O58" s="47">
+        <v>10</v>
+      </c>
+      <c r="P58" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q58" s="47">
+        <v>6</v>
+      </c>
+      <c r="R58" s="43" t="s">
+        <v>111</v>
+      </c>
       <c r="S58" s="11"/>
       <c r="T58" s="11"/>
       <c r="U58" s="11"/>
@@ -31561,9 +32000,17 @@
       <c r="AB999" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="F47:J47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="O47:R47"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>